<commit_message>
priority rule to be smarter
</commit_message>
<xml_diff>
--- a/NameListSample.xlsx
+++ b/NameListSample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23715" windowHeight="11895"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23715" windowHeight="11895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="671">
   <si>
     <t>王眾慧</t>
   </si>
@@ -2042,10 +2042,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>iphone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PS4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2059,6 +2055,25 @@
   </si>
   <si>
     <t>5000元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600元</t>
+  </si>
+  <si>
+    <t>600元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iPhone Xs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -17120,8 +17135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -19783,10 +19798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -19804,7 +19819,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>662</v>
+        <v>670</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -19828,7 +19843,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -19836,7 +19851,87 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>